<commit_message>
fix save error on the long description
</commit_message>
<xml_diff>
--- a/Document/Gestione errori.xlsx
+++ b/Document/Gestione errori.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0091D7-58DC-4E08-A707-0044205C0004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE9CD70-7C66-4C7E-9B2D-1EAC55CA3565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t xml:space="preserve">MODULO </t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>da verificare</t>
+  </si>
+  <si>
+    <t>spese annuali</t>
+  </si>
+  <si>
+    <t>non salva nel db le note e non midifica colore del pannello</t>
+  </si>
+  <si>
+    <t>verificare inserimento</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,6 +703,23 @@
         <v>44879</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44883</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>